<commit_message>
First successful package created
</commit_message>
<xml_diff>
--- a/SourceDocuments/InPut_Excel/Time_Stamp.xlsx
+++ b/SourceDocuments/InPut_Excel/Time_Stamp.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="195">
   <si>
     <t>index1_5s_A</t>
   </si>
@@ -376,6 +376,231 @@
   </si>
   <si>
     <t>index3_1d_A</t>
+  </si>
+  <si>
+    <t>index4_5s_A</t>
+  </si>
+  <si>
+    <t>index5_5s_A</t>
+  </si>
+  <si>
+    <t>"091800"</t>
+  </si>
+  <si>
+    <t>"092800"</t>
+  </si>
+  <si>
+    <t>"093800"</t>
+  </si>
+  <si>
+    <t>"094800"</t>
+  </si>
+  <si>
+    <t>"095800"</t>
+  </si>
+  <si>
+    <t>"100800"</t>
+  </si>
+  <si>
+    <t>"101800"</t>
+  </si>
+  <si>
+    <t>"102800"</t>
+  </si>
+  <si>
+    <t>"103800"</t>
+  </si>
+  <si>
+    <t>"104800"</t>
+  </si>
+  <si>
+    <t>"105800"</t>
+  </si>
+  <si>
+    <t>"110800"</t>
+  </si>
+  <si>
+    <t>"111800"</t>
+  </si>
+  <si>
+    <t>"112800"</t>
+  </si>
+  <si>
+    <t>"113800"</t>
+  </si>
+  <si>
+    <t>"114800"</t>
+  </si>
+  <si>
+    <t>"093400"</t>
+  </si>
+  <si>
+    <t>"094400"</t>
+  </si>
+  <si>
+    <t>"095400"</t>
+  </si>
+  <si>
+    <t>"100400"</t>
+  </si>
+  <si>
+    <t>"101400"</t>
+  </si>
+  <si>
+    <t>"102400"</t>
+  </si>
+  <si>
+    <t>"103400"</t>
+  </si>
+  <si>
+    <t>"104400"</t>
+  </si>
+  <si>
+    <t>"105400"</t>
+  </si>
+  <si>
+    <t>"110400"</t>
+  </si>
+  <si>
+    <t>"111400"</t>
+  </si>
+  <si>
+    <t>"112400"</t>
+  </si>
+  <si>
+    <t>"113400"</t>
+  </si>
+  <si>
+    <t>"114400"</t>
+  </si>
+  <si>
+    <t>"115400"</t>
+  </si>
+  <si>
+    <t>"120400"</t>
+  </si>
+  <si>
+    <t>index4_5s_B</t>
+  </si>
+  <si>
+    <t>index5_5s_B</t>
+  </si>
+  <si>
+    <t>"080000"</t>
+  </si>
+  <si>
+    <t>"083000"</t>
+  </si>
+  <si>
+    <t>"090000"</t>
+  </si>
+  <si>
+    <t>"093000"</t>
+  </si>
+  <si>
+    <t>"100000"</t>
+  </si>
+  <si>
+    <t>"103000"</t>
+  </si>
+  <si>
+    <t>"110000"</t>
+  </si>
+  <si>
+    <t>"113000"</t>
+  </si>
+  <si>
+    <t>"120000"</t>
+  </si>
+  <si>
+    <t>index4_1m_A</t>
+  </si>
+  <si>
+    <t>index5_1m_A</t>
+  </si>
+  <si>
+    <t>"091900"</t>
+  </si>
+  <si>
+    <t>"112000"</t>
+  </si>
+  <si>
+    <t>"132000"</t>
+  </si>
+  <si>
+    <t>"152000"</t>
+  </si>
+  <si>
+    <t>"172800"</t>
+  </si>
+  <si>
+    <t>"040000"</t>
+  </si>
+  <si>
+    <t>"055500"</t>
+  </si>
+  <si>
+    <t>"075500"</t>
+  </si>
+  <si>
+    <t>"085500"</t>
+  </si>
+  <si>
+    <t>"115100"</t>
+  </si>
+  <si>
+    <t>"135200"</t>
+  </si>
+  <si>
+    <t>"155200"</t>
+  </si>
+  <si>
+    <t>"175200"</t>
+  </si>
+  <si>
+    <t>"200000"</t>
+  </si>
+  <si>
+    <t>"063300"</t>
+  </si>
+  <si>
+    <t>"082800"</t>
+  </si>
+  <si>
+    <t>index4_5m_A</t>
+  </si>
+  <si>
+    <t>index5_5m_A</t>
+  </si>
+  <si>
+    <t>"084500"</t>
+  </si>
+  <si>
+    <t>"120500"</t>
+  </si>
+  <si>
+    <t>"115500"</t>
+  </si>
+  <si>
+    <t>"164000"</t>
+  </si>
+  <si>
+    <t>index4_30m_A</t>
+  </si>
+  <si>
+    <t>index5_30m_A</t>
+  </si>
+  <si>
+    <t>index4_1h_A</t>
+  </si>
+  <si>
+    <t>index5_1h_A</t>
+  </si>
+  <si>
+    <t>index4_1d_A</t>
+  </si>
+  <si>
+    <t>index5_1d_A</t>
   </si>
 </sst>
 </file>
@@ -731,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM19"/>
+  <dimension ref="A1:BI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AU27" sqref="AU27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,38 +970,57 @@
     <col min="4" max="4" width="3.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.28515625" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
+    <col min="11" max="11" width="3.5703125" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.28515625" customWidth="1"/>
-    <col min="14" max="14" width="3.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.28515625" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.28515625" customWidth="1"/>
-    <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.28515625" customWidth="1"/>
-    <col min="21" max="21" width="3.5703125" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.28515625" customWidth="1"/>
-    <col min="24" max="24" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.28515625" customWidth="1"/>
-    <col min="26" max="26" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.28515625" customWidth="1"/>
-    <col min="28" max="28" width="3.5703125" customWidth="1"/>
-    <col min="29" max="30" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="3.5703125" customWidth="1"/>
-    <col min="33" max="34" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.28515625" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.28515625" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.28515625" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.28515625" customWidth="1"/>
+    <col min="22" max="22" width="3.5703125" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.28515625" customWidth="1"/>
+    <col min="25" max="25" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.28515625" customWidth="1"/>
+    <col min="27" max="27" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.28515625" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.28515625" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="3.28515625" customWidth="1"/>
+    <col min="33" max="33" width="3.5703125" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3.28515625" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.28515625" customWidth="1"/>
+    <col min="38" max="38" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="3.28515625" customWidth="1"/>
+    <col min="40" max="40" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="3.28515625" customWidth="1"/>
+    <col min="42" max="42" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="3.28515625" customWidth="1"/>
+    <col min="44" max="44" width="3.5703125" customWidth="1"/>
+    <col min="45" max="46" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="3.5703125" customWidth="1"/>
+    <col min="51" max="52" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -786,68 +1030,110 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" t="s">
+      <c r="G1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
+        <v>154</v>
+      </c>
+      <c r="T1" t="s">
+        <v>155</v>
+      </c>
+      <c r="V1" s="2"/>
+      <c r="W1" t="s">
         <v>72</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Y1" t="s">
         <v>73</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AA1" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="2"/>
-      <c r="V1" t="s">
+      <c r="AC1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AG1" s="2"/>
+      <c r="AH1" t="s">
         <v>100</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AJ1" t="s">
         <v>101</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AL1" t="s">
         <v>102</v>
       </c>
-      <c r="AB1" s="2"/>
-      <c r="AC1" t="s">
+      <c r="AN1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AR1" s="2"/>
+      <c r="AS1" t="s">
         <v>110</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AT1" t="s">
         <v>111</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AU1" t="s">
         <v>112</v>
       </c>
-      <c r="AF1" s="2"/>
-      <c r="AG1" t="s">
+      <c r="AV1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AX1" s="2"/>
+      <c r="AY1" t="s">
         <v>114</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AZ1" t="s">
         <v>115</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="BA1" t="s">
         <v>116</v>
       </c>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" t="s">
+      <c r="BB1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BD1" s="2"/>
+      <c r="BE1" t="s">
         <v>117</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="BF1" t="s">
         <v>118</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="BG1" t="s">
         <v>119</v>
       </c>
+      <c r="BH1" t="s">
+        <v>193</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>194</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -866,95 +1152,161 @@
       <c r="F2" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" t="s">
+        <v>122</v>
+      </c>
       <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" t="s">
         <v>38</v>
       </c>
-      <c r="I2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" t="s">
         <v>39</v>
       </c>
-      <c r="K2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
         <v>63</v>
       </c>
-      <c r="M2" t="s">
-        <v>71</v>
-      </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" t="s">
+        <v>156</v>
+      </c>
+      <c r="S2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" t="s">
+        <v>157</v>
+      </c>
+      <c r="U2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" s="2"/>
+      <c r="W2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="P2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="X2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" t="s">
         <v>84</v>
       </c>
-      <c r="R2" t="s">
-        <v>71</v>
-      </c>
-      <c r="S2" s="1" t="s">
+      <c r="Z2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="T2" t="s">
-        <v>71</v>
-      </c>
-      <c r="U2" s="2"/>
-      <c r="V2" t="s">
+      <c r="AB2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG2" s="2"/>
+      <c r="AH2" t="s">
         <v>80</v>
       </c>
-      <c r="W2" t="s">
-        <v>71</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="AI2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>105</v>
       </c>
-      <c r="Y2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AK2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL2" t="s">
         <v>107</v>
       </c>
-      <c r="AA2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB2" s="2"/>
-      <c r="AC2" t="s">
+      <c r="AM2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>187</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR2" s="2"/>
+      <c r="AS2" t="s">
         <v>80</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AT2" t="s">
         <v>88</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AU2" t="s">
         <v>113</v>
       </c>
-      <c r="AF2" s="2"/>
-      <c r="AG2" t="s">
+      <c r="AV2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AX2" s="2"/>
+      <c r="AY2" t="s">
         <v>80</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AZ2" t="s">
         <v>88</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="BA2" t="s">
         <v>113</v>
       </c>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" t="s">
+      <c r="BB2" t="s">
+        <v>172</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>180</v>
+      </c>
+      <c r="BD2" s="2"/>
+      <c r="BE2" t="s">
         <v>80</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="BF2" t="s">
         <v>88</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="BG2" t="s">
         <v>113</v>
       </c>
+      <c r="BH2" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>180</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -973,68 +1325,116 @@
       <c r="F3" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" t="s">
+        <v>123</v>
+      </c>
       <c r="H3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" t="s">
         <v>39</v>
       </c>
-      <c r="I3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" t="s">
         <v>40</v>
       </c>
-      <c r="K3" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P3" t="s">
         <v>64</v>
       </c>
-      <c r="M3" t="s">
-        <v>71</v>
-      </c>
-      <c r="N3" s="2"/>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R3" t="s">
+        <v>157</v>
+      </c>
+      <c r="S3" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" t="s">
+        <v>158</v>
+      </c>
+      <c r="U3" t="s">
+        <v>71</v>
+      </c>
+      <c r="V3" s="2"/>
+      <c r="W3" t="s">
         <v>75</v>
       </c>
-      <c r="P3" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="X3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y3" t="s">
         <v>85</v>
       </c>
-      <c r="R3" t="s">
-        <v>71</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="Z3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA3" t="s">
         <v>93</v>
       </c>
-      <c r="T3" t="s">
-        <v>71</v>
-      </c>
-      <c r="U3" s="2"/>
-      <c r="V3" t="s">
+      <c r="AB3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG3" s="2"/>
+      <c r="AH3" t="s">
         <v>103</v>
       </c>
-      <c r="W3" t="s">
-        <v>71</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="AI3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ3" t="s">
         <v>106</v>
       </c>
-      <c r="Y3" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="AK3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL3" t="s">
         <v>108</v>
       </c>
-      <c r="AA3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AJ3" s="2"/>
+      <c r="AM3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>185</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>188</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="BD3" s="2"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1053,68 +1453,116 @@
       <c r="F4" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" t="s">
+        <v>124</v>
+      </c>
       <c r="H4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" t="s">
         <v>40</v>
       </c>
-      <c r="I4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N4" t="s">
         <v>41</v>
       </c>
-      <c r="K4" t="s">
-        <v>71</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P4" t="s">
         <v>65</v>
       </c>
-      <c r="M4" t="s">
-        <v>71</v>
-      </c>
-      <c r="N4" s="2"/>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
+        <v>71</v>
+      </c>
+      <c r="R4" t="s">
+        <v>158</v>
+      </c>
+      <c r="S4" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" t="s">
+        <v>159</v>
+      </c>
+      <c r="U4" t="s">
+        <v>71</v>
+      </c>
+      <c r="V4" s="2"/>
+      <c r="W4" t="s">
         <v>76</v>
       </c>
-      <c r="P4" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="X4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y4" t="s">
         <v>86</v>
       </c>
-      <c r="R4" t="s">
-        <v>71</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="Z4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA4" t="s">
         <v>94</v>
       </c>
-      <c r="T4" t="s">
-        <v>71</v>
-      </c>
-      <c r="U4" s="2"/>
-      <c r="V4" t="s">
+      <c r="AB4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG4" s="2"/>
+      <c r="AH4" t="s">
         <v>104</v>
       </c>
-      <c r="W4" t="s">
-        <v>71</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="AI4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>88</v>
       </c>
-      <c r="Y4" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="AK4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL4" t="s">
         <v>109</v>
       </c>
-      <c r="AA4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AJ4" s="2"/>
+      <c r="AM4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="BD4" s="2"/>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1133,59 +1581,101 @@
       <c r="F5" t="s">
         <v>71</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" t="s">
+        <v>125</v>
+      </c>
       <c r="H5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" t="s">
         <v>41</v>
       </c>
-      <c r="I5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="M5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N5" t="s">
         <v>42</v>
       </c>
-      <c r="K5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="O5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P5" t="s">
         <v>66</v>
       </c>
-      <c r="M5" t="s">
-        <v>71</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
+        <v>71</v>
+      </c>
+      <c r="R5" t="s">
+        <v>159</v>
+      </c>
+      <c r="S5" t="s">
+        <v>71</v>
+      </c>
+      <c r="T5" t="s">
+        <v>160</v>
+      </c>
+      <c r="U5" t="s">
+        <v>71</v>
+      </c>
+      <c r="V5" s="2"/>
+      <c r="W5" t="s">
         <v>78</v>
       </c>
-      <c r="P5" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="X5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y5" t="s">
         <v>87</v>
       </c>
-      <c r="R5" t="s">
-        <v>71</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="Z5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA5" t="s">
         <v>95</v>
       </c>
-      <c r="T5" t="s">
-        <v>71</v>
-      </c>
-      <c r="U5" s="2"/>
-      <c r="V5" t="s">
+      <c r="AB5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>179</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG5" s="2"/>
+      <c r="AH5" t="s">
         <v>78</v>
       </c>
-      <c r="X5" t="s">
+      <c r="AJ5" t="s">
         <v>87</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AL5" t="s">
         <v>95</v>
       </c>
-      <c r="AB5" s="2"/>
-      <c r="AF5" s="2"/>
-      <c r="AJ5" s="2"/>
+      <c r="AN5" t="s">
+        <v>170</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>179</v>
+      </c>
+      <c r="AR5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="BD5" s="2"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1204,50 +1694,86 @@
       <c r="F6" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" t="s">
+        <v>126</v>
+      </c>
       <c r="H6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" t="s">
+        <v>142</v>
+      </c>
+      <c r="J6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" t="s">
         <v>42</v>
       </c>
-      <c r="I6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="M6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" t="s">
         <v>43</v>
       </c>
-      <c r="K6" t="s">
-        <v>71</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="O6" t="s">
+        <v>71</v>
+      </c>
+      <c r="P6" t="s">
         <v>67</v>
       </c>
-      <c r="M6" t="s">
-        <v>71</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R6" t="s">
+        <v>160</v>
+      </c>
+      <c r="S6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T6" t="s">
+        <v>161</v>
+      </c>
+      <c r="U6" t="s">
+        <v>71</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="W6" t="s">
         <v>79</v>
       </c>
-      <c r="P6" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="X6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y6" t="s">
         <v>88</v>
       </c>
-      <c r="R6" t="s">
-        <v>71</v>
-      </c>
-      <c r="S6" t="s">
+      <c r="Z6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA6" t="s">
         <v>96</v>
       </c>
-      <c r="T6" t="s">
-        <v>71</v>
-      </c>
-      <c r="U6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AF6" s="2"/>
-      <c r="AJ6" s="2"/>
+      <c r="AB6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="BD6" s="2"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1266,50 +1792,86 @@
       <c r="F7" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" t="s">
+        <v>127</v>
+      </c>
       <c r="H7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" t="s">
         <v>43</v>
       </c>
-      <c r="I7" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="M7" t="s">
+        <v>71</v>
+      </c>
+      <c r="N7" t="s">
         <v>44</v>
       </c>
-      <c r="K7" t="s">
-        <v>71</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="O7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P7" t="s">
         <v>68</v>
       </c>
-      <c r="M7" t="s">
-        <v>71</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
+        <v>71</v>
+      </c>
+      <c r="R7" t="s">
+        <v>161</v>
+      </c>
+      <c r="S7" t="s">
+        <v>71</v>
+      </c>
+      <c r="T7" t="s">
+        <v>162</v>
+      </c>
+      <c r="U7" t="s">
+        <v>71</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="W7" t="s">
         <v>80</v>
       </c>
-      <c r="P7" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="X7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y7" t="s">
         <v>89</v>
       </c>
-      <c r="R7" t="s">
-        <v>71</v>
-      </c>
-      <c r="S7" t="s">
+      <c r="Z7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA7" t="s">
         <v>97</v>
       </c>
-      <c r="T7" t="s">
-        <v>71</v>
-      </c>
-      <c r="U7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AJ7" s="2"/>
+      <c r="AB7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AX7" s="2"/>
+      <c r="BD7" s="2"/>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1328,50 +1890,86 @@
       <c r="F8" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" t="s">
+        <v>128</v>
+      </c>
       <c r="H8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" t="s">
+        <v>144</v>
+      </c>
+      <c r="J8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" t="s">
         <v>44</v>
       </c>
-      <c r="I8" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="M8" t="s">
+        <v>71</v>
+      </c>
+      <c r="N8" t="s">
         <v>45</v>
       </c>
-      <c r="K8" t="s">
-        <v>71</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="O8" t="s">
+        <v>71</v>
+      </c>
+      <c r="P8" t="s">
         <v>69</v>
       </c>
-      <c r="M8" t="s">
-        <v>71</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" t="s">
+      <c r="Q8" t="s">
+        <v>71</v>
+      </c>
+      <c r="R8" t="s">
+        <v>162</v>
+      </c>
+      <c r="S8" t="s">
+        <v>71</v>
+      </c>
+      <c r="T8" t="s">
+        <v>163</v>
+      </c>
+      <c r="U8" t="s">
+        <v>71</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" t="s">
         <v>81</v>
       </c>
-      <c r="P8" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="X8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y8" t="s">
         <v>90</v>
       </c>
-      <c r="R8" t="s">
-        <v>71</v>
-      </c>
-      <c r="S8" t="s">
+      <c r="Z8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA8" t="s">
         <v>98</v>
       </c>
-      <c r="T8" t="s">
-        <v>71</v>
-      </c>
-      <c r="U8" s="2"/>
-      <c r="AB8" s="2"/>
-      <c r="AF8" s="2"/>
-      <c r="AJ8" s="2"/>
+      <c r="AB8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="BD8" s="2"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1390,41 +1988,71 @@
       <c r="F9" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" t="s">
+        <v>129</v>
+      </c>
       <c r="H9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" t="s">
+        <v>145</v>
+      </c>
+      <c r="J9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" t="s">
         <v>45</v>
       </c>
-      <c r="J9" t="s">
+      <c r="N9" t="s">
         <v>46</v>
       </c>
-      <c r="L9" t="s">
+      <c r="P9" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" t="s">
+      <c r="R9" t="s">
+        <v>163</v>
+      </c>
+      <c r="T9" t="s">
+        <v>164</v>
+      </c>
+      <c r="V9" s="2"/>
+      <c r="W9" t="s">
         <v>82</v>
       </c>
-      <c r="P9" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="X9" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y9" t="s">
         <v>10</v>
       </c>
-      <c r="R9" t="s">
-        <v>71</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="Z9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA9" t="s">
         <v>99</v>
       </c>
-      <c r="T9" t="s">
-        <v>71</v>
-      </c>
-      <c r="U9" s="2"/>
-      <c r="AB9" s="2"/>
-      <c r="AF9" s="2"/>
-      <c r="AJ9" s="2"/>
+      <c r="AB9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="BD9" s="2"/>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1443,23 +2071,41 @@
       <c r="F10" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" t="s">
+      <c r="G10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" t="s">
         <v>83</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Y10" t="s">
         <v>16</v>
       </c>
-      <c r="S10" t="s">
+      <c r="AA10" t="s">
         <v>91</v>
       </c>
-      <c r="U10" s="2"/>
-      <c r="AB10" s="2"/>
-      <c r="AF10" s="2"/>
-      <c r="AJ10" s="2"/>
+      <c r="AC10" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG10" s="2"/>
+      <c r="AR10" s="2"/>
+      <c r="AX10" s="2"/>
+      <c r="BD10" s="2"/>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1478,14 +2124,26 @@
       <c r="F11" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="AB11" s="2"/>
-      <c r="AF11" s="2"/>
-      <c r="AJ11" s="2"/>
+      <c r="G11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="BD11" s="2"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1504,14 +2162,26 @@
       <c r="F12" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="AB12" s="2"/>
-      <c r="AF12" s="2"/>
-      <c r="AJ12" s="2"/>
+      <c r="G12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" t="s">
+        <v>148</v>
+      </c>
+      <c r="J12" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="BD12" s="2"/>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1530,14 +2200,26 @@
       <c r="F13" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AF13" s="2"/>
-      <c r="AJ13" s="2"/>
+      <c r="G13" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AR13" s="2"/>
+      <c r="AX13" s="2"/>
+      <c r="BD13" s="2"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1556,14 +2238,26 @@
       <c r="F14" t="s">
         <v>71</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AF14" s="2"/>
-      <c r="AJ14" s="2"/>
+      <c r="G14" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="BD14" s="2"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1582,14 +2276,26 @@
       <c r="F15" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="AB15" s="2"/>
-      <c r="AF15" s="2"/>
-      <c r="AJ15" s="2"/>
+      <c r="G15" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="AG15" s="2"/>
+      <c r="AR15" s="2"/>
+      <c r="AX15" s="2"/>
+      <c r="BD15" s="2"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1608,15 +2314,28 @@
       <c r="F16" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="Q16" s="3"/>
-      <c r="U16" s="2"/>
-      <c r="AB16" s="2"/>
-      <c r="AF16" s="2"/>
-      <c r="AJ16" s="2"/>
+      <c r="G16" t="s">
+        <v>136</v>
+      </c>
+      <c r="H16" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="Y16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AG16" s="2"/>
+      <c r="AR16" s="2"/>
+      <c r="AX16" s="2"/>
+      <c r="BD16" s="2"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1635,15 +2354,22 @@
       <c r="F17" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="AB17" s="2"/>
-      <c r="AF17" s="2"/>
-      <c r="AJ17" s="2"/>
+      <c r="G17" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AR17" s="2"/>
+      <c r="AX17" s="2"/>
+      <c r="BD17" s="2"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="O19" s="3"/>
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="W19" s="3"/>
+      <c r="AC19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
0x12. JavaScript - Warm up
</commit_message>
<xml_diff>
--- a/SourceDocuments/InPut_Excel/Time_Stamp.xlsx
+++ b/SourceDocuments/InPut_Excel/Time_Stamp.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Ver1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="467">
   <si>
     <t>index1_5s_A</t>
   </si>
@@ -601,13 +601,829 @@
   </si>
   <si>
     <t>index5_1d_A</t>
+  </si>
+  <si>
+    <t>"09:55:00"</t>
+  </si>
+  <si>
+    <t>"12:28:00"</t>
+  </si>
+  <si>
+    <t>"16:28:00"</t>
+  </si>
+  <si>
+    <t>"14:28:00"</t>
+  </si>
+  <si>
+    <t>"13:55:00"</t>
+  </si>
+  <si>
+    <t>"15:55:00"</t>
+  </si>
+  <si>
+    <t>"18:28:00"</t>
+  </si>
+  <si>
+    <t>"095500"</t>
+  </si>
+  <si>
+    <t>"135500"</t>
+  </si>
+  <si>
+    <t>"155500"</t>
+  </si>
+  <si>
+    <t>"122800"</t>
+  </si>
+  <si>
+    <t>"142800"</t>
+  </si>
+  <si>
+    <t>"162800"</t>
+  </si>
+  <si>
+    <t>"182800"</t>
+  </si>
+  <si>
+    <t>"095500_to_122800"</t>
+  </si>
+  <si>
+    <t>"115500_to_142800"</t>
+  </si>
+  <si>
+    <t>"135500_to_162800"</t>
+  </si>
+  <si>
+    <t>"155500_to_182800"</t>
+  </si>
+  <si>
+    <t>"08:31:00"</t>
+  </si>
+  <si>
+    <t>"09:01:00"</t>
+  </si>
+  <si>
+    <t>"09:31:00"</t>
+  </si>
+  <si>
+    <t>"10:01:00"</t>
+  </si>
+  <si>
+    <t>"10:31:00"</t>
+  </si>
+  <si>
+    <t>"11:01:00"</t>
+  </si>
+  <si>
+    <t>"11:31:00"</t>
+  </si>
+  <si>
+    <t>"12:01:00"</t>
+  </si>
+  <si>
+    <t>"07:59:00"</t>
+  </si>
+  <si>
+    <t>"08:29:00"</t>
+  </si>
+  <si>
+    <t>"08:59:00"</t>
+  </si>
+  <si>
+    <t>"09:29:00"</t>
+  </si>
+  <si>
+    <t>"09:59:00"</t>
+  </si>
+  <si>
+    <t>"10:29:00"</t>
+  </si>
+  <si>
+    <t>"10:59:00"</t>
+  </si>
+  <si>
+    <t>"11:29:00"</t>
+  </si>
+  <si>
+    <t>"075900"</t>
+  </si>
+  <si>
+    <t>"082900"</t>
+  </si>
+  <si>
+    <t>"085900"</t>
+  </si>
+  <si>
+    <t>"092900"</t>
+  </si>
+  <si>
+    <t>"095900"</t>
+  </si>
+  <si>
+    <t>"102900"</t>
+  </si>
+  <si>
+    <t>"105900"</t>
+  </si>
+  <si>
+    <t>"112900"</t>
+  </si>
+  <si>
+    <t>"083100"</t>
+  </si>
+  <si>
+    <t>"090100"</t>
+  </si>
+  <si>
+    <t>"093100"</t>
+  </si>
+  <si>
+    <t>"100100"</t>
+  </si>
+  <si>
+    <t>"103100"</t>
+  </si>
+  <si>
+    <t>"110100"</t>
+  </si>
+  <si>
+    <t>"113100"</t>
+  </si>
+  <si>
+    <t>"120100"</t>
+  </si>
+  <si>
+    <t>"075900_to_083100"</t>
+  </si>
+  <si>
+    <t>"082900_to_090100"</t>
+  </si>
+  <si>
+    <t>"085900_to_093100"</t>
+  </si>
+  <si>
+    <t>"092900_to_100100"</t>
+  </si>
+  <si>
+    <t>"095900_to_103100"</t>
+  </si>
+  <si>
+    <t>"102900_to_110100"</t>
+  </si>
+  <si>
+    <t>"105900_to_113100"</t>
+  </si>
+  <si>
+    <t>"112900_to_120100"</t>
+  </si>
+  <si>
+    <t>"11:58:00"</t>
+  </si>
+  <si>
+    <t>"12:14:00"</t>
+  </si>
+  <si>
+    <t>"115800"</t>
+  </si>
+  <si>
+    <t>"121400"</t>
+  </si>
+  <si>
+    <t>"115800_to_121400"</t>
+  </si>
+  <si>
+    <t>09:28:00</t>
+  </si>
+  <si>
+    <t>09:18:00</t>
+  </si>
+  <si>
+    <t>09:38:00</t>
+  </si>
+  <si>
+    <t>09:48:00</t>
+  </si>
+  <si>
+    <t>09:58:00</t>
+  </si>
+  <si>
+    <t>10:08:00</t>
+  </si>
+  <si>
+    <t>10:18:00</t>
+  </si>
+  <si>
+    <t>10:28:00</t>
+  </si>
+  <si>
+    <t>10:38:00</t>
+  </si>
+  <si>
+    <t>10:48:00</t>
+  </si>
+  <si>
+    <t>10:58:00</t>
+  </si>
+  <si>
+    <t>11:08:00</t>
+  </si>
+  <si>
+    <t>11:18:00</t>
+  </si>
+  <si>
+    <t>11:28:00</t>
+  </si>
+  <si>
+    <t>11:38:00</t>
+  </si>
+  <si>
+    <t>11:48:00</t>
+  </si>
+  <si>
+    <t>11:58:00</t>
+  </si>
+  <si>
+    <t>10:01:00</t>
+  </si>
+  <si>
+    <t>09:34:00</t>
+  </si>
+  <si>
+    <t>09:44:00</t>
+  </si>
+  <si>
+    <t>09:54:00</t>
+  </si>
+  <si>
+    <t>10:04:00</t>
+  </si>
+  <si>
+    <t>10:14:00</t>
+  </si>
+  <si>
+    <t>10:24:00</t>
+  </si>
+  <si>
+    <t>10:34:00</t>
+  </si>
+  <si>
+    <t>10:44:00</t>
+  </si>
+  <si>
+    <t>10:54:00</t>
+  </si>
+  <si>
+    <t>11:04:00</t>
+  </si>
+  <si>
+    <t>11:14:00</t>
+  </si>
+  <si>
+    <t>11:24:00</t>
+  </si>
+  <si>
+    <t>11:34:00</t>
+  </si>
+  <si>
+    <t>11:44:00</t>
+  </si>
+  <si>
+    <t>11:54:00</t>
+  </si>
+  <si>
+    <t>12:04:00</t>
+  </si>
+  <si>
+    <t>12:14:00</t>
+  </si>
+  <si>
+    <t>intraday</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>-0.41</t>
+  </si>
+  <si>
+    <t>MarketOpen</t>
+  </si>
+  <si>
+    <t>07:59:00</t>
+  </si>
+  <si>
+    <t>08:29:00</t>
+  </si>
+  <si>
+    <t>08:59:00</t>
+  </si>
+  <si>
+    <t>09:29:00</t>
+  </si>
+  <si>
+    <t>09:59:00</t>
+  </si>
+  <si>
+    <t>10:29:00</t>
+  </si>
+  <si>
+    <t>10:59:00</t>
+  </si>
+  <si>
+    <t>11:29:00</t>
+  </si>
+  <si>
+    <t>08:31:00</t>
+  </si>
+  <si>
+    <t>09:01:00</t>
+  </si>
+  <si>
+    <t>09:31:00</t>
+  </si>
+  <si>
+    <t>10:31:00</t>
+  </si>
+  <si>
+    <t>11:01:00</t>
+  </si>
+  <si>
+    <t>11:31:00</t>
+  </si>
+  <si>
+    <t>12:01:00</t>
+  </si>
+  <si>
+    <t>091800_to_093400</t>
+  </si>
+  <si>
+    <t>092800_to_094400</t>
+  </si>
+  <si>
+    <t>093800_to_095400</t>
+  </si>
+  <si>
+    <t>094800_to_100400</t>
+  </si>
+  <si>
+    <t>095800_to_101400</t>
+  </si>
+  <si>
+    <t>100800_to_102400</t>
+  </si>
+  <si>
+    <t>101800_to_103400</t>
+  </si>
+  <si>
+    <t>102800_to_104400</t>
+  </si>
+  <si>
+    <t>103800_to_105400</t>
+  </si>
+  <si>
+    <t>104800_to_110400</t>
+  </si>
+  <si>
+    <t>105800_to_111400</t>
+  </si>
+  <si>
+    <t>110800_to_112400</t>
+  </si>
+  <si>
+    <t>111800_to_113400</t>
+  </si>
+  <si>
+    <t>112800_to_114400</t>
+  </si>
+  <si>
+    <t>113800_to_115400</t>
+  </si>
+  <si>
+    <t>114800_to_120400</t>
+  </si>
+  <si>
+    <t>115800_to_121400</t>
+  </si>
+  <si>
+    <t>075900_to_083100</t>
+  </si>
+  <si>
+    <t>082900_to_090100</t>
+  </si>
+  <si>
+    <t>085900_to_093100</t>
+  </si>
+  <si>
+    <t>092900_to_100100</t>
+  </si>
+  <si>
+    <t>095900_to_103100</t>
+  </si>
+  <si>
+    <t>102900_to_110100</t>
+  </si>
+  <si>
+    <t>105900_to_113100</t>
+  </si>
+  <si>
+    <t>112900_to_120100</t>
+  </si>
+  <si>
+    <t>092800_to_100000</t>
+  </si>
+  <si>
+    <t>Index1_</t>
+  </si>
+  <si>
+    <t>Index2_</t>
+  </si>
+  <si>
+    <t>Name_</t>
+  </si>
+  <si>
+    <t>Fibonacci_</t>
+  </si>
+  <si>
+    <t>Scope_</t>
+  </si>
+  <si>
+    <t>HourConstant_</t>
+  </si>
+  <si>
+    <t>MinConstant_</t>
+  </si>
+  <si>
+    <t>SecConstant_</t>
+  </si>
+  <si>
+    <t>leftSide_</t>
+  </si>
+  <si>
+    <t>Blank_</t>
+  </si>
+  <si>
+    <t>Index1_5s</t>
+  </si>
+  <si>
+    <t>Index2_5s</t>
+  </si>
+  <si>
+    <t>Name_5s</t>
+  </si>
+  <si>
+    <t>Fibonacci_5s</t>
+  </si>
+  <si>
+    <t>Scope_5s</t>
+  </si>
+  <si>
+    <t>HourConstant_5s</t>
+  </si>
+  <si>
+    <t>MinConstant_5s</t>
+  </si>
+  <si>
+    <t>SecConstant_5s</t>
+  </si>
+  <si>
+    <t>leftSide_5s</t>
+  </si>
+  <si>
+    <t>Blank_5s</t>
+  </si>
+  <si>
+    <t>Index1_1m</t>
+  </si>
+  <si>
+    <t>Index2_1m</t>
+  </si>
+  <si>
+    <t>Name_1m</t>
+  </si>
+  <si>
+    <t>Fibonacci_1m</t>
+  </si>
+  <si>
+    <t>Scope_1m</t>
+  </si>
+  <si>
+    <t>HourConstant_1m</t>
+  </si>
+  <si>
+    <t>MinConstant_1m</t>
+  </si>
+  <si>
+    <t>SecConstant_1m</t>
+  </si>
+  <si>
+    <t>leftSide_1m</t>
+  </si>
+  <si>
+    <t>Blank_1m</t>
+  </si>
+  <si>
+    <t>09:19:00</t>
+  </si>
+  <si>
+    <t>04:00:00</t>
+  </si>
+  <si>
+    <t>05:55:00</t>
+  </si>
+  <si>
+    <t>07:55:00</t>
+  </si>
+  <si>
+    <t>09:55:00</t>
+  </si>
+  <si>
+    <t>11:55:00</t>
+  </si>
+  <si>
+    <t>13:55:00</t>
+  </si>
+  <si>
+    <t>15:55:00</t>
+  </si>
+  <si>
+    <t>17:28:00</t>
+  </si>
+  <si>
+    <t>11:51:00</t>
+  </si>
+  <si>
+    <t>06:33:00</t>
+  </si>
+  <si>
+    <t>08:28:00</t>
+  </si>
+  <si>
+    <t>12:28:00</t>
+  </si>
+  <si>
+    <t>14:28:00</t>
+  </si>
+  <si>
+    <t>16:28:00</t>
+  </si>
+  <si>
+    <t>18:28:00</t>
+  </si>
+  <si>
+    <t>20:00:00</t>
+  </si>
+  <si>
+    <t>091900_to_115100</t>
+  </si>
+  <si>
+    <t>040000_to_063300</t>
+  </si>
+  <si>
+    <t>055500_to_082800</t>
+  </si>
+  <si>
+    <t>075500_to_102800</t>
+  </si>
+  <si>
+    <t>095500_to_122800</t>
+  </si>
+  <si>
+    <t>115500_to_142800</t>
+  </si>
+  <si>
+    <t>135500_to_162800</t>
+  </si>
+  <si>
+    <t>155500_to_182800</t>
+  </si>
+  <si>
+    <t>172800_to_200000</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>-0.35</t>
+  </si>
+  <si>
+    <t>Index1_5m</t>
+  </si>
+  <si>
+    <t>Index2_5m</t>
+  </si>
+  <si>
+    <t>Name_5m</t>
+  </si>
+  <si>
+    <t>Fibonacci_5m</t>
+  </si>
+  <si>
+    <t>Scope_5m</t>
+  </si>
+  <si>
+    <t>HourConstant_5m</t>
+  </si>
+  <si>
+    <t>MinConstant_5m</t>
+  </si>
+  <si>
+    <t>SecConstant_5m</t>
+  </si>
+  <si>
+    <t>leftSide_5m</t>
+  </si>
+  <si>
+    <t>Blank_5m</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>-0.36</t>
+  </si>
+  <si>
+    <t>040000_to_115500</t>
+  </si>
+  <si>
+    <t>084500_to_164000</t>
+  </si>
+  <si>
+    <t>120500_to_200000</t>
+  </si>
+  <si>
+    <t>Index1_30m</t>
+  </si>
+  <si>
+    <t>Index2_30m</t>
+  </si>
+  <si>
+    <t>Name_30m</t>
+  </si>
+  <si>
+    <t>Fibonacci_30m</t>
+  </si>
+  <si>
+    <t>Scope_30m</t>
+  </si>
+  <si>
+    <t>HourConstant_30m</t>
+  </si>
+  <si>
+    <t>MinConstant_30m</t>
+  </si>
+  <si>
+    <t>SecConstant_30m</t>
+  </si>
+  <si>
+    <t>leftSide_30m</t>
+  </si>
+  <si>
+    <t>Blank_30m</t>
+  </si>
+  <si>
+    <t>040000_to_200000</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>-0.38</t>
+  </si>
+  <si>
+    <t>Index1_1h</t>
+  </si>
+  <si>
+    <t>Index2_1h</t>
+  </si>
+  <si>
+    <t>Name_1h</t>
+  </si>
+  <si>
+    <t>Fibonacci_1h</t>
+  </si>
+  <si>
+    <t>Scope_1h</t>
+  </si>
+  <si>
+    <t>HourConstant_1h</t>
+  </si>
+  <si>
+    <t>MinConstant_1h</t>
+  </si>
+  <si>
+    <t>SecConstant_1h</t>
+  </si>
+  <si>
+    <t>leftSide_1h</t>
+  </si>
+  <si>
+    <t>Blank_1h</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>-0.51</t>
+  </si>
+  <si>
+    <t>Index1_1d</t>
+  </si>
+  <si>
+    <t>Index2_1d</t>
+  </si>
+  <si>
+    <t>Name_1d</t>
+  </si>
+  <si>
+    <t>Fibonacci_1d</t>
+  </si>
+  <si>
+    <t>Scope_1d</t>
+  </si>
+  <si>
+    <t>HourConstant_1d</t>
+  </si>
+  <si>
+    <t>MinConstant_1d</t>
+  </si>
+  <si>
+    <t>SecConstant_1d</t>
+  </si>
+  <si>
+    <t>leftSide_1d</t>
+  </si>
+  <si>
+    <t>Blank_1d</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>StartDelta_5s</t>
+  </si>
+  <si>
+    <t>EndDelta_5s</t>
+  </si>
+  <si>
+    <t>StartDelta_1m</t>
+  </si>
+  <si>
+    <t>EndDelta_1m</t>
+  </si>
+  <si>
+    <t>StartDelta_5m</t>
+  </si>
+  <si>
+    <t>EndDelta_5m</t>
+  </si>
+  <si>
+    <t>StartDelta_30m</t>
+  </si>
+  <si>
+    <t>EndDelta_30m</t>
+  </si>
+  <si>
+    <t>StartDelta_1h</t>
+  </si>
+  <si>
+    <t>EndDelta_1h</t>
+  </si>
+  <si>
+    <t>StartDelta_</t>
+  </si>
+  <si>
+    <t>EndDelta_</t>
+  </si>
+  <si>
+    <t>StartDelta_1d</t>
+  </si>
+  <si>
+    <t>EndDelta_1d</t>
+  </si>
+  <si>
+    <t>08:45:00</t>
+  </si>
+  <si>
+    <t>12:05:00</t>
+  </si>
+  <si>
+    <t>16:40:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20:00:00 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -615,14 +1431,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCCCCCC"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,6 +1442,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,13 +1464,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -956,10 +1772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BI19"/>
+  <dimension ref="A1:BJ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AU27" sqref="AU27"/>
+    <sheetView topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BE1" sqref="BE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1836,7 @@
     <col min="60" max="61" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1132,8 +1948,9 @@
       <c r="BI1" t="s">
         <v>194</v>
       </c>
+      <c r="BJ1" s="2"/>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1305,8 +2122,9 @@
       <c r="BI2" t="s">
         <v>180</v>
       </c>
+      <c r="BJ2" s="2"/>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1433,8 +2251,9 @@
       <c r="AR3" s="2"/>
       <c r="AX3" s="2"/>
       <c r="BD3" s="2"/>
+      <c r="BJ3" s="2"/>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1561,8 +2380,9 @@
       <c r="AR4" s="2"/>
       <c r="AX4" s="2"/>
       <c r="BD4" s="2"/>
+      <c r="BJ4" s="2"/>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1674,8 +2494,9 @@
       <c r="AR5" s="2"/>
       <c r="AX5" s="2"/>
       <c r="BD5" s="2"/>
+      <c r="BJ5" s="2"/>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1772,8 +2593,9 @@
       <c r="AR6" s="2"/>
       <c r="AX6" s="2"/>
       <c r="BD6" s="2"/>
+      <c r="BJ6" s="2"/>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1870,8 +2692,9 @@
       <c r="AR7" s="2"/>
       <c r="AX7" s="2"/>
       <c r="BD7" s="2"/>
+      <c r="BJ7" s="2"/>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1968,8 +2791,9 @@
       <c r="AR8" s="2"/>
       <c r="AX8" s="2"/>
       <c r="BD8" s="2"/>
+      <c r="BJ8" s="2"/>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2051,8 +2875,9 @@
       <c r="AR9" s="2"/>
       <c r="AX9" s="2"/>
       <c r="BD9" s="2"/>
+      <c r="BJ9" s="2"/>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2104,8 +2929,9 @@
       <c r="AR10" s="2"/>
       <c r="AX10" s="2"/>
       <c r="BD10" s="2"/>
+      <c r="BJ10" s="2"/>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2142,8 +2968,9 @@
       <c r="AR11" s="2"/>
       <c r="AX11" s="2"/>
       <c r="BD11" s="2"/>
+      <c r="BJ11" s="2"/>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2180,8 +3007,9 @@
       <c r="AR12" s="2"/>
       <c r="AX12" s="2"/>
       <c r="BD12" s="2"/>
+      <c r="BJ12" s="2"/>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2218,8 +3046,9 @@
       <c r="AR13" s="2"/>
       <c r="AX13" s="2"/>
       <c r="BD13" s="2"/>
+      <c r="BJ13" s="2"/>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2256,8 +3085,9 @@
       <c r="AR14" s="2"/>
       <c r="AX14" s="2"/>
       <c r="BD14" s="2"/>
+      <c r="BJ14" s="2"/>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2294,8 +3124,9 @@
       <c r="AR15" s="2"/>
       <c r="AX15" s="2"/>
       <c r="BD15" s="2"/>
+      <c r="BJ15" s="2"/>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2328,14 +3159,13 @@
       </c>
       <c r="K16" s="2"/>
       <c r="V16" s="2"/>
-      <c r="Y16" s="3"/>
-      <c r="AE16" s="3"/>
       <c r="AG16" s="2"/>
       <c r="AR16" s="2"/>
       <c r="AX16" s="2"/>
       <c r="BD16" s="2"/>
+      <c r="BJ16" s="2"/>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2366,10 +3196,1194 @@
       <c r="AR17" s="2"/>
       <c r="AX17" s="2"/>
       <c r="BD17" s="2"/>
+      <c r="BJ17" s="2"/>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="W19" s="3"/>
-      <c r="AC19" s="3"/>
+    <row r="18" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2"/>
+      <c r="AK18" s="2"/>
+      <c r="AL18" s="2"/>
+      <c r="AM18" s="2"/>
+      <c r="AN18" s="2"/>
+      <c r="AO18" s="2"/>
+      <c r="AP18" s="2"/>
+      <c r="AQ18" s="2"/>
+      <c r="AR18" s="2"/>
+      <c r="AS18" s="2"/>
+      <c r="AT18" s="2"/>
+      <c r="AU18" s="2"/>
+      <c r="AV18" s="2"/>
+      <c r="AW18" s="2"/>
+      <c r="AX18" s="2"/>
+      <c r="AY18" s="2"/>
+      <c r="AZ18" s="2"/>
+      <c r="BA18" s="2"/>
+      <c r="BB18" s="2"/>
+      <c r="BC18" s="2"/>
+      <c r="BD18" s="2"/>
+      <c r="BE18" s="2"/>
+      <c r="BF18" s="2"/>
+      <c r="BG18" s="2"/>
+      <c r="BH18" s="2"/>
+      <c r="BI18" s="2"/>
+      <c r="BJ18" s="2"/>
+    </row>
+    <row r="19" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="2"/>
+      <c r="AK19" s="2"/>
+      <c r="AL19" s="2"/>
+      <c r="AM19" s="2"/>
+      <c r="AN19" s="2"/>
+      <c r="AO19" s="2"/>
+      <c r="AP19" s="2"/>
+      <c r="AQ19" s="2"/>
+      <c r="AR19" s="2"/>
+      <c r="AS19" s="2"/>
+      <c r="AT19" s="2"/>
+      <c r="AU19" s="2"/>
+      <c r="AV19" s="2"/>
+      <c r="AW19" s="2"/>
+      <c r="AX19" s="2"/>
+      <c r="AY19" s="2"/>
+      <c r="AZ19" s="2"/>
+      <c r="BA19" s="2"/>
+      <c r="BB19" s="2"/>
+      <c r="BC19" s="2"/>
+      <c r="BD19" s="2"/>
+      <c r="BE19" s="2"/>
+      <c r="BF19" s="2"/>
+      <c r="BG19" s="2"/>
+      <c r="BH19" s="2"/>
+      <c r="BI19" s="2"/>
+      <c r="BJ19" s="2"/>
+    </row>
+    <row r="22" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>216</v>
+      </c>
+      <c r="D22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" t="s">
+        <v>159</v>
+      </c>
+      <c r="H22" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" t="s">
+        <v>160</v>
+      </c>
+      <c r="J22" t="s">
+        <v>71</v>
+      </c>
+      <c r="L22" t="s">
+        <v>221</v>
+      </c>
+      <c r="M22" t="s">
+        <v>71</v>
+      </c>
+      <c r="N22" t="s">
+        <v>213</v>
+      </c>
+      <c r="O22" t="s">
+        <v>71</v>
+      </c>
+      <c r="P22" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>71</v>
+      </c>
+      <c r="R22" t="s">
+        <v>229</v>
+      </c>
+      <c r="S22" t="s">
+        <v>71</v>
+      </c>
+      <c r="T22" t="s">
+        <v>237</v>
+      </c>
+      <c r="U22" t="s">
+        <v>71</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="X22" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" t="s">
+        <v>122</v>
+      </c>
+      <c r="H23" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" t="s">
+        <v>138</v>
+      </c>
+      <c r="J23" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" t="s">
+        <v>222</v>
+      </c>
+      <c r="M23" t="s">
+        <v>71</v>
+      </c>
+      <c r="N23" t="s">
+        <v>214</v>
+      </c>
+      <c r="O23" t="s">
+        <v>71</v>
+      </c>
+      <c r="P23" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>71</v>
+      </c>
+      <c r="R23" t="s">
+        <v>230</v>
+      </c>
+      <c r="S23" t="s">
+        <v>71</v>
+      </c>
+      <c r="T23" t="s">
+        <v>238</v>
+      </c>
+      <c r="U23" t="s">
+        <v>71</v>
+      </c>
+      <c r="W23" t="s">
+        <v>80</v>
+      </c>
+      <c r="X23" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" t="s">
+        <v>123</v>
+      </c>
+      <c r="H24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" t="s">
+        <v>139</v>
+      </c>
+      <c r="J24" t="s">
+        <v>71</v>
+      </c>
+      <c r="L24" t="s">
+        <v>223</v>
+      </c>
+      <c r="M24" t="s">
+        <v>71</v>
+      </c>
+      <c r="N24" t="s">
+        <v>215</v>
+      </c>
+      <c r="O24" t="s">
+        <v>71</v>
+      </c>
+      <c r="P24" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>71</v>
+      </c>
+      <c r="R24" t="s">
+        <v>231</v>
+      </c>
+      <c r="S24" t="s">
+        <v>71</v>
+      </c>
+      <c r="T24" t="s">
+        <v>239</v>
+      </c>
+      <c r="U24" t="s">
+        <v>71</v>
+      </c>
+      <c r="W24" t="s">
+        <v>81</v>
+      </c>
+      <c r="X24" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" t="s">
+        <v>124</v>
+      </c>
+      <c r="H25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" t="s">
+        <v>140</v>
+      </c>
+      <c r="J25" t="s">
+        <v>71</v>
+      </c>
+      <c r="L25" t="s">
+        <v>224</v>
+      </c>
+      <c r="M25" t="s">
+        <v>71</v>
+      </c>
+      <c r="N25" t="s">
+        <v>216</v>
+      </c>
+      <c r="O25" t="s">
+        <v>71</v>
+      </c>
+      <c r="P25" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>71</v>
+      </c>
+      <c r="R25" t="s">
+        <v>232</v>
+      </c>
+      <c r="S25" t="s">
+        <v>71</v>
+      </c>
+      <c r="T25" t="s">
+        <v>240</v>
+      </c>
+      <c r="U25" t="s">
+        <v>71</v>
+      </c>
+      <c r="W25" t="s">
+        <v>82</v>
+      </c>
+      <c r="X25" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" t="s">
+        <v>141</v>
+      </c>
+      <c r="J26" t="s">
+        <v>71</v>
+      </c>
+      <c r="L26" t="s">
+        <v>225</v>
+      </c>
+      <c r="M26" t="s">
+        <v>71</v>
+      </c>
+      <c r="N26" t="s">
+        <v>217</v>
+      </c>
+      <c r="O26" t="s">
+        <v>71</v>
+      </c>
+      <c r="P26" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>71</v>
+      </c>
+      <c r="R26" t="s">
+        <v>233</v>
+      </c>
+      <c r="S26" t="s">
+        <v>71</v>
+      </c>
+      <c r="T26" t="s">
+        <v>241</v>
+      </c>
+      <c r="U26" t="s">
+        <v>71</v>
+      </c>
+      <c r="W26" t="s">
+        <v>195</v>
+      </c>
+      <c r="X26" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>209</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>205</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I27" t="s">
+        <v>142</v>
+      </c>
+      <c r="J27" t="s">
+        <v>71</v>
+      </c>
+      <c r="L27" t="s">
+        <v>226</v>
+      </c>
+      <c r="M27" t="s">
+        <v>71</v>
+      </c>
+      <c r="N27" t="s">
+        <v>218</v>
+      </c>
+      <c r="O27" t="s">
+        <v>71</v>
+      </c>
+      <c r="P27" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>71</v>
+      </c>
+      <c r="R27" t="s">
+        <v>234</v>
+      </c>
+      <c r="S27" t="s">
+        <v>71</v>
+      </c>
+      <c r="T27" t="s">
+        <v>242</v>
+      </c>
+      <c r="U27" t="s">
+        <v>71</v>
+      </c>
+      <c r="W27" t="s">
+        <v>105</v>
+      </c>
+      <c r="X27" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>210</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" t="s">
+        <v>127</v>
+      </c>
+      <c r="H28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I28" t="s">
+        <v>143</v>
+      </c>
+      <c r="J28" t="s">
+        <v>71</v>
+      </c>
+      <c r="L28" t="s">
+        <v>227</v>
+      </c>
+      <c r="M28" t="s">
+        <v>71</v>
+      </c>
+      <c r="N28" t="s">
+        <v>219</v>
+      </c>
+      <c r="O28" t="s">
+        <v>71</v>
+      </c>
+      <c r="P28" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>71</v>
+      </c>
+      <c r="R28" t="s">
+        <v>235</v>
+      </c>
+      <c r="S28" t="s">
+        <v>71</v>
+      </c>
+      <c r="T28" t="s">
+        <v>243</v>
+      </c>
+      <c r="U28" t="s">
+        <v>71</v>
+      </c>
+      <c r="W28" t="s">
+        <v>199</v>
+      </c>
+      <c r="X28" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>211</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" t="s">
+        <v>128</v>
+      </c>
+      <c r="H29" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" t="s">
+        <v>144</v>
+      </c>
+      <c r="J29" t="s">
+        <v>71</v>
+      </c>
+      <c r="L29" t="s">
+        <v>228</v>
+      </c>
+      <c r="N29" t="s">
+        <v>220</v>
+      </c>
+      <c r="P29" t="s">
+        <v>252</v>
+      </c>
+      <c r="R29" t="s">
+        <v>236</v>
+      </c>
+      <c r="T29" t="s">
+        <v>244</v>
+      </c>
+      <c r="W29" t="s">
+        <v>200</v>
+      </c>
+      <c r="X29" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>212</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" t="s">
+        <v>129</v>
+      </c>
+      <c r="H30" t="s">
+        <v>71</v>
+      </c>
+      <c r="I30" t="s">
+        <v>145</v>
+      </c>
+      <c r="J30" t="s">
+        <v>71</v>
+      </c>
+      <c r="W30" t="s">
+        <v>79</v>
+      </c>
+      <c r="X30" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" t="s">
+        <v>130</v>
+      </c>
+      <c r="H31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I31" t="s">
+        <v>146</v>
+      </c>
+      <c r="J31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" t="s">
+        <v>131</v>
+      </c>
+      <c r="H32" t="s">
+        <v>71</v>
+      </c>
+      <c r="I32" t="s">
+        <v>147</v>
+      </c>
+      <c r="J32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" t="s">
+        <v>132</v>
+      </c>
+      <c r="H33" t="s">
+        <v>71</v>
+      </c>
+      <c r="I33" t="s">
+        <v>148</v>
+      </c>
+      <c r="J33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H34" t="s">
+        <v>71</v>
+      </c>
+      <c r="I34" t="s">
+        <v>149</v>
+      </c>
+      <c r="J34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F35" t="s">
+        <v>71</v>
+      </c>
+      <c r="G35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H35" t="s">
+        <v>71</v>
+      </c>
+      <c r="I35" t="s">
+        <v>150</v>
+      </c>
+      <c r="J35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" t="s">
+        <v>135</v>
+      </c>
+      <c r="H36" t="s">
+        <v>71</v>
+      </c>
+      <c r="I36" t="s">
+        <v>151</v>
+      </c>
+      <c r="J36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" t="s">
+        <v>136</v>
+      </c>
+      <c r="H37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" t="s">
+        <v>137</v>
+      </c>
+      <c r="H38" t="s">
+        <v>71</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>253</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E39" t="s">
+        <v>257</v>
+      </c>
+      <c r="F39" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" t="s">
+        <v>255</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>256</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2379,13 +4393,1980 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:CF27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AD10" sqref="AD10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="73" max="74" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="9.140625" style="3"/>
+    <col min="80" max="80" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="85" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="AX1" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="AY1" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="AZ1" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="BA1" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="BB1" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="BC1" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="BD1" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="BE1" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="BF1" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="BG1" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="BH1" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="BI1" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="BK1" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="BT1" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="CA1" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="CB1" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="CC1" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="CD1" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="CE1" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="CF1" s="4" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="P2" s="5">
+        <v>-1</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>-1</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>409</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="AN2" s="5">
+        <v>-6</v>
+      </c>
+      <c r="AO2" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AP2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="AZ2" s="5">
+        <v>-21</v>
+      </c>
+      <c r="BA2" s="5">
+        <v>-1</v>
+      </c>
+      <c r="BB2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="BE2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="BG2" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="BI2" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="BJ2" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="BK2" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="BL2" s="5">
+        <v>-220</v>
+      </c>
+      <c r="BM2" s="5">
+        <v>-1</v>
+      </c>
+      <c r="BN2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="BO2" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="BP2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="BQ2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="BR2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="BS2" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="BX2" s="5"/>
+      <c r="BY2" s="5"/>
+      <c r="BZ2" s="3"/>
+    </row>
+    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="P3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="R3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>410</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="3"/>
+      <c r="AZ3" s="5"/>
+      <c r="BA3" s="5"/>
+      <c r="BB3" s="3"/>
+      <c r="BL3" s="5"/>
+      <c r="BM3" s="5"/>
+      <c r="BN3" s="3"/>
+      <c r="BX3" s="5"/>
+      <c r="BY3" s="5"/>
+      <c r="BZ3" s="3"/>
+    </row>
+    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="P4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="R4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>411</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AD4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="3"/>
+      <c r="AZ4" s="5"/>
+      <c r="BA4" s="5"/>
+      <c r="BB4" s="3"/>
+      <c r="BL4" s="5"/>
+      <c r="BM4" s="5"/>
+      <c r="BN4" s="3"/>
+      <c r="BX4" s="5"/>
+      <c r="BY4" s="5"/>
+      <c r="BZ4" s="3"/>
+    </row>
+    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="P5" s="5">
+        <v>-1</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>-1</v>
+      </c>
+      <c r="R5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="3"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="3"/>
+      <c r="AZ5" s="5"/>
+      <c r="BA5" s="5"/>
+      <c r="BB5" s="3"/>
+      <c r="BL5" s="5"/>
+      <c r="BM5" s="5"/>
+      <c r="BN5" s="3"/>
+      <c r="BX5" s="5"/>
+      <c r="BY5" s="5"/>
+      <c r="BZ5" s="3"/>
+    </row>
+    <row r="6" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="P6" s="5">
+        <v>-1</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>-1</v>
+      </c>
+      <c r="R6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="3"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="3"/>
+      <c r="AZ6" s="5"/>
+      <c r="BA6" s="5"/>
+      <c r="BB6" s="3"/>
+      <c r="BL6" s="5"/>
+      <c r="BM6" s="5"/>
+      <c r="BN6" s="3"/>
+      <c r="BX6" s="5"/>
+      <c r="BY6" s="5"/>
+      <c r="BZ6" s="3"/>
+    </row>
+    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="P7" s="5">
+        <v>-1</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>-1</v>
+      </c>
+      <c r="R7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="3"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="3"/>
+      <c r="AZ7" s="5"/>
+      <c r="BA7" s="5"/>
+      <c r="BB7" s="3"/>
+      <c r="BL7" s="5"/>
+      <c r="BM7" s="5"/>
+      <c r="BN7" s="3"/>
+      <c r="BX7" s="5"/>
+      <c r="BY7" s="5"/>
+      <c r="BZ7" s="3"/>
+    </row>
+    <row r="8" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="P8" s="5">
+        <v>-1</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>-1</v>
+      </c>
+      <c r="R8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="3"/>
+      <c r="AN8" s="5"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="3"/>
+      <c r="AZ8" s="5"/>
+      <c r="BA8" s="5"/>
+      <c r="BB8" s="3"/>
+      <c r="BL8" s="5"/>
+      <c r="BM8" s="5"/>
+      <c r="BN8" s="3"/>
+      <c r="BX8" s="5"/>
+      <c r="BY8" s="5"/>
+      <c r="BZ8" s="3"/>
+    </row>
+    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="P9" s="5">
+        <v>-1</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>-1</v>
+      </c>
+      <c r="R9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="3"/>
+      <c r="AN9" s="5"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="3"/>
+      <c r="AZ9" s="5"/>
+      <c r="BA9" s="5"/>
+      <c r="BB9" s="3"/>
+      <c r="BL9" s="5"/>
+      <c r="BM9" s="5"/>
+      <c r="BN9" s="3"/>
+      <c r="BX9" s="5"/>
+      <c r="BY9" s="5"/>
+      <c r="BZ9" s="3"/>
+    </row>
+    <row r="10" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="P10" s="5">
+        <v>-1</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>-1</v>
+      </c>
+      <c r="R10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="3"/>
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="3"/>
+      <c r="AZ10" s="5"/>
+      <c r="BA10" s="5"/>
+      <c r="BB10" s="3"/>
+      <c r="BL10" s="5"/>
+      <c r="BM10" s="5"/>
+      <c r="BN10" s="3"/>
+      <c r="BX10" s="5"/>
+      <c r="BY10" s="5"/>
+      <c r="BZ10" s="3"/>
+    </row>
+    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R11" s="3"/>
+      <c r="Z11" s="1"/>
+      <c r="AD11" s="3"/>
+      <c r="AP11" s="3"/>
+      <c r="BB11" s="3"/>
+      <c r="BN11" s="3"/>
+      <c r="BZ11" s="3"/>
+    </row>
+    <row r="12" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R12" s="3"/>
+      <c r="Z12" s="1"/>
+      <c r="AD12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="BB12" s="3"/>
+      <c r="BN12" s="3"/>
+      <c r="BZ12" s="3"/>
+    </row>
+    <row r="13" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R13" s="3"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AD13" s="3"/>
+      <c r="AP13" s="3"/>
+      <c r="BB13" s="3"/>
+      <c r="BN13" s="3"/>
+      <c r="BZ13" s="3"/>
+    </row>
+    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R14" s="3"/>
+      <c r="Y14" s="1"/>
+      <c r="AD14" s="3"/>
+      <c r="AP14" s="3"/>
+      <c r="BB14" s="3"/>
+      <c r="BN14" s="3"/>
+      <c r="BZ14" s="3"/>
+    </row>
+    <row r="15" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R15" s="3"/>
+      <c r="Y15" s="1"/>
+      <c r="AD15" s="3"/>
+      <c r="AP15" s="3"/>
+      <c r="BB15" s="3"/>
+      <c r="BN15" s="3"/>
+      <c r="BZ15" s="3"/>
+    </row>
+    <row r="16" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="AD16" s="3"/>
+      <c r="AP16" s="3"/>
+      <c r="BB16" s="3"/>
+      <c r="BN16" s="3"/>
+      <c r="BZ16" s="3"/>
+    </row>
+    <row r="17" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AP17" s="3"/>
+      <c r="BB17" s="3"/>
+      <c r="BN17" s="3"/>
+      <c r="BZ17" s="3"/>
+    </row>
+    <row r="18" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AP18" s="3"/>
+      <c r="BB18" s="3"/>
+      <c r="BN18" s="3"/>
+      <c r="BZ18" s="3"/>
+    </row>
+    <row r="19" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AP19" s="3"/>
+      <c r="BB19" s="3"/>
+      <c r="BN19" s="3"/>
+      <c r="BZ19" s="3"/>
+    </row>
+    <row r="20" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AP20" s="3"/>
+      <c r="BB20" s="3"/>
+      <c r="BN20" s="3"/>
+      <c r="BZ20" s="3"/>
+    </row>
+    <row r="21" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AP21" s="3"/>
+      <c r="BB21" s="3"/>
+      <c r="BN21" s="3"/>
+      <c r="BZ21" s="3"/>
+    </row>
+    <row r="22" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F22" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AP22" s="3"/>
+      <c r="BB22" s="3"/>
+      <c r="BN22" s="3"/>
+      <c r="BZ22" s="3"/>
+    </row>
+    <row r="23" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AP23" s="3"/>
+      <c r="BB23" s="3"/>
+      <c r="BN23" s="3"/>
+      <c r="BZ23" s="3"/>
+    </row>
+    <row r="24" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AP24" s="3"/>
+      <c r="BB24" s="3"/>
+      <c r="BN24" s="3"/>
+      <c r="BZ24" s="3"/>
+    </row>
+    <row r="25" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F25" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AP25" s="3"/>
+      <c r="BB25" s="3"/>
+      <c r="BN25" s="3"/>
+      <c r="BZ25" s="3"/>
+    </row>
+    <row r="26" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F26" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AP26" s="3"/>
+      <c r="BB26" s="3"/>
+      <c r="BN26" s="3"/>
+      <c r="BZ26" s="3"/>
+    </row>
+    <row r="27" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F27" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AP27" s="3"/>
+      <c r="BB27" s="3"/>
+      <c r="BN27" s="3"/>
+      <c r="BZ27" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
{New commit drop here}
</commit_message>
<xml_diff>
--- a/SourceDocuments/InPut_Excel/Time_Stamp.xlsx
+++ b/SourceDocuments/InPut_Excel/Time_Stamp.xlsx
@@ -4395,8 +4395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AD10" sqref="AD10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>